<commit_message>
fewer spaces for reading CO to save time
also excel with updated schedule number
</commit_message>
<xml_diff>
--- a/Resources/1-Validation.xlsx
+++ b/Resources/1-Validation.xlsx
@@ -321,8 +321,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="false"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="false"/>
+        <i val="false"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="false" table="false" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
 </styleSheet>
 </file>
 
@@ -615,7 +643,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -860,7 +888,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -873,7 +901,7 @@
         <v>49</v>
       </c>
       <c r="B1">
-        <v>138</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
After Run, schedule counter update in excel
</commit_message>
<xml_diff>
--- a/Resources/1-Validation.xlsx
+++ b/Resources/1-Validation.xlsx
@@ -643,7 +643,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -901,7 +901,7 @@
         <v>49</v>
       </c>
       <c r="B1">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
updated  changes to 8-expanding invoice validation
</commit_message>
<xml_diff>
--- a/Resources/1-Validation.xlsx
+++ b/Resources/1-Validation.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8115" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8115" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" fullCalcOnLoad="true"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="84">
   <si>
     <t>Invoice No</t>
   </si>
@@ -181,9 +181,6 @@
   </si>
   <si>
     <t>DeliveryNumber</t>
-  </si>
-  <si>
-    <t>3013691711</t>
   </si>
   <si>
     <t>1000004200</t>
@@ -276,8 +273,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,8 +312,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -325,7 +322,7 @@
     <dxf>
       <font>
         <b/>
-        <i val="false"/>
+        <i val="0"/>
       </font>
       <fill>
         <patternFill>
@@ -335,8 +332,8 @@
     </dxf>
     <dxf>
       <font>
-        <b val="false"/>
-        <i val="false"/>
+        <b val="0"/>
+        <i val="0"/>
       </font>
       <fill>
         <patternFill patternType="none">
@@ -346,11 +343,16 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="false" table="false" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -397,7 +399,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -449,7 +451,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -650,40 +652,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="12.5703125" bestFit="true" customWidth="true"/>
-    <col min="3" max="3" width="10.42578125" bestFit="true" customWidth="true"/>
-    <col min="4" max="4" width="12" bestFit="true" customWidth="true"/>
-    <col min="5" max="5" width="14.28515625" bestFit="true" customWidth="true"/>
-    <col min="6" max="6" width="10.7109375" bestFit="true" customWidth="true"/>
-    <col min="7" max="7" width="4.85546875" bestFit="true" customWidth="true"/>
-    <col min="8" max="8" width="15.28515625" bestFit="true" customWidth="true"/>
-    <col min="9" max="9" width="12.42578125" bestFit="true" customWidth="true"/>
-    <col min="10" max="10" width="16.140625" bestFit="true" customWidth="true"/>
-    <col min="11" max="11" width="28.42578125" bestFit="true" customWidth="true"/>
-    <col min="12" max="12" width="25.28515625" bestFit="true" customWidth="true"/>
-    <col min="13" max="13" width="14.85546875" bestFit="true" customWidth="true"/>
-    <col min="14" max="14" width="16" bestFit="true" customWidth="true"/>
-    <col min="15" max="15" width="17.28515625" bestFit="true" customWidth="true"/>
-    <col min="16" max="16" width="22.5703125" bestFit="true" customWidth="true"/>
-    <col min="17" max="17" width="16.85546875" bestFit="true" customWidth="true"/>
-    <col min="18" max="18" width="25.140625" bestFit="true" customWidth="true"/>
-    <col min="19" max="19" width="15.140625" bestFit="true" customWidth="true"/>
-    <col min="20" max="20" width="11.7109375" bestFit="true" customWidth="true"/>
-    <col min="21" max="21" width="13.42578125" bestFit="true" customWidth="true"/>
-    <col min="22" max="22" width="27" bestFit="true" customWidth="true"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -751,7 +753,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3013684370</v>
       </c>
@@ -819,7 +821,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K3" t="s">
         <v>23</v>
       </c>
@@ -830,7 +832,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K4" t="s">
         <v>24</v>
       </c>
@@ -841,7 +843,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K5" t="s">
         <v>25</v>
       </c>
@@ -852,27 +854,27 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="U10" t="s">
         <v>46</v>
       </c>
@@ -884,19 +886,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" bestFit="true" customWidth="true"/>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -904,7 +906,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -918,22 +920,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="11.42578125" bestFit="true" customWidth="true"/>
-    <col min="3" max="3" width="16.5703125" bestFit="true" customWidth="true"/>
-    <col min="4" max="4" width="15.85546875" bestFit="true" customWidth="true"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -947,144 +949,144 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3013691711</v>
+      </c>
+      <c r="B2" t="s">
         <v>55</v>
-      </c>
-      <c r="B2" t="s">
-        <v>56</v>
       </c>
       <c r="C2">
         <v>21708102017</v>
       </c>
       <c r="D2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>58</v>
-      </c>
-      <c r="B3" t="s">
-        <v>59</v>
       </c>
       <c r="C3">
         <v>22008102017</v>
       </c>
       <c r="D3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>61</v>
-      </c>
-      <c r="B4" t="s">
-        <v>62</v>
       </c>
       <c r="C4">
         <v>22108102017</v>
       </c>
       <c r="D4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>64</v>
-      </c>
-      <c r="B5" t="s">
-        <v>65</v>
       </c>
       <c r="C5">
         <v>22208102017</v>
       </c>
       <c r="D5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>67</v>
-      </c>
-      <c r="B6" t="s">
-        <v>68</v>
       </c>
       <c r="C6">
         <v>22308102017</v>
       </c>
       <c r="D6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>70</v>
-      </c>
-      <c r="B7" t="s">
-        <v>71</v>
       </c>
       <c r="C7">
         <v>22408102017</v>
       </c>
       <c r="D7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>73</v>
-      </c>
-      <c r="B8" t="s">
-        <v>74</v>
       </c>
       <c r="C8">
         <v>22608102017</v>
       </c>
       <c r="D8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>76</v>
-      </c>
-      <c r="B9" t="s">
-        <v>77</v>
       </c>
       <c r="C9">
         <v>22708102017</v>
       </c>
       <c r="D9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>79</v>
-      </c>
-      <c r="B10" t="s">
-        <v>80</v>
       </c>
       <c r="C10">
         <v>22808102017</v>
       </c>
       <c r="D10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>82</v>
-      </c>
-      <c r="B11" t="s">
-        <v>83</v>
       </c>
       <c r="C11">
         <v>22908102017</v>
       </c>
       <c r="D11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Read or Write Data to Excel
</commit_message>
<xml_diff>
--- a/Resources/1-Validation.xlsx
+++ b/Resources/1-Validation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="98">
   <si>
     <t>Invoice No</t>
   </si>
@@ -271,6 +271,45 @@
   </si>
   <si>
     <t>13141502</t>
+  </si>
+  <si>
+    <t>3013696612</t>
+  </si>
+  <si>
+    <t>1000004634</t>
+  </si>
+  <si>
+    <t>schedNum</t>
+  </si>
+  <si>
+    <t>13187320</t>
+  </si>
+  <si>
+    <t>3013696615</t>
+  </si>
+  <si>
+    <t>1000004635</t>
+  </si>
+  <si>
+    <t>13187327</t>
+  </si>
+  <si>
+    <t>3013696616</t>
+  </si>
+  <si>
+    <t>1000004636</t>
+  </si>
+  <si>
+    <t>13187330</t>
+  </si>
+  <si>
+    <t>3013696618</t>
+  </si>
+  <si>
+    <t>1000004637</t>
+  </si>
+  <si>
+    <t>13187333</t>
   </si>
 </sst>
 </file>
@@ -901,7 +940,7 @@
         <v>49</v>
       </c>
       <c r="B1">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2">
@@ -909,7 +948,7 @@
         <v>50</v>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -919,7 +958,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D3"/>
@@ -1087,6 +1126,62 @@
         <v>84</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" t="s">
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Image update for Configuration
</commit_message>
<xml_diff>
--- a/Resources/1-Validation.xlsx
+++ b/Resources/1-Validation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="120">
   <si>
     <t>Invoice No</t>
   </si>
@@ -367,6 +367,15 @@
   </si>
   <si>
     <t>1000004646</t>
+  </si>
+  <si>
+    <t>3013696628</t>
+  </si>
+  <si>
+    <t>1000004650</t>
+  </si>
+  <si>
+    <t>13188908</t>
   </si>
 </sst>
 </file>
@@ -997,7 +1006,7 @@
         <v>49</v>
       </c>
       <c r="B1">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2">
@@ -1005,7 +1014,7 @@
         <v>50</v>
       </c>
       <c r="B2">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1015,7 +1024,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D3"/>
@@ -1337,6 +1346,20 @@
         <v>114</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>117</v>
+      </c>
+      <c r="B23" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
1-add 13 to bad data, reset start point to line #2
also update schedule number
</commit_message>
<xml_diff>
--- a/Resources/1-Validation.xlsx
+++ b/Resources/1-Validation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="159">
   <si>
     <t>Invoice No</t>
   </si>
@@ -412,6 +412,87 @@
   </si>
   <si>
     <t>13188995</t>
+  </si>
+  <si>
+    <t>3013696736</t>
+  </si>
+  <si>
+    <t>1000004664</t>
+  </si>
+  <si>
+    <t>13190563</t>
+  </si>
+  <si>
+    <t>3013696737</t>
+  </si>
+  <si>
+    <t>1000004665</t>
+  </si>
+  <si>
+    <t>13190565</t>
+  </si>
+  <si>
+    <t>3013696739</t>
+  </si>
+  <si>
+    <t>1000004667</t>
+  </si>
+  <si>
+    <t>13190569</t>
+  </si>
+  <si>
+    <t>3013696742</t>
+  </si>
+  <si>
+    <t>1000004669</t>
+  </si>
+  <si>
+    <t>13190573</t>
+  </si>
+  <si>
+    <t>3013696745</t>
+  </si>
+  <si>
+    <t>1000004671</t>
+  </si>
+  <si>
+    <t>13190576</t>
+  </si>
+  <si>
+    <t>3013696746</t>
+  </si>
+  <si>
+    <t>1000004672</t>
+  </si>
+  <si>
+    <t>13190579</t>
+  </si>
+  <si>
+    <t>3013696747</t>
+  </si>
+  <si>
+    <t>1000004673</t>
+  </si>
+  <si>
+    <t>13190581</t>
+  </si>
+  <si>
+    <t>3013696748</t>
+  </si>
+  <si>
+    <t>1000004674</t>
+  </si>
+  <si>
+    <t>13190583</t>
+  </si>
+  <si>
+    <t>3013696749</t>
+  </si>
+  <si>
+    <t>1000004675</t>
+  </si>
+  <si>
+    <t>13190585</t>
   </si>
 </sst>
 </file>
@@ -784,7 +865,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1042,7 +1123,7 @@
         <v>49</v>
       </c>
       <c r="B1">
-        <v>122</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2">
@@ -1050,7 +1131,7 @@
         <v>50</v>
       </c>
       <c r="B2">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1060,7 +1141,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D3"/>
@@ -1452,6 +1533,132 @@
         <v>131</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28" t="s">
+        <v>133</v>
+      </c>
+      <c r="C28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" t="s">
+        <v>136</v>
+      </c>
+      <c r="C29" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>138</v>
+      </c>
+      <c r="B30" t="s">
+        <v>139</v>
+      </c>
+      <c r="C30" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>141</v>
+      </c>
+      <c r="B31" t="s">
+        <v>142</v>
+      </c>
+      <c r="C31" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>144</v>
+      </c>
+      <c r="B32" t="s">
+        <v>145</v>
+      </c>
+      <c r="C32" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>147</v>
+      </c>
+      <c r="B33" t="s">
+        <v>148</v>
+      </c>
+      <c r="C33" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>150</v>
+      </c>
+      <c r="B34" t="s">
+        <v>151</v>
+      </c>
+      <c r="C34" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>153</v>
+      </c>
+      <c r="B35" t="s">
+        <v>154</v>
+      </c>
+      <c r="C35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>156</v>
+      </c>
+      <c r="B36" t="s">
+        <v>157</v>
+      </c>
+      <c r="C36" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" t="s">
+        <v>158</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated script8 with new dataset
</commit_message>
<xml_diff>
--- a/Resources/1-Validation.xlsx
+++ b/Resources/1-Validation.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8115" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8115" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="139">
   <si>
     <t>Invoice No</t>
   </si>
@@ -427,19 +428,39 @@
   </si>
   <si>
     <t>13190571</t>
+  </si>
+  <si>
+    <t>InvoiceNo</t>
+  </si>
+  <si>
+    <t>COnumber</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -469,10 +490,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -815,7 +841,7 @@
   <dimension ref="A1:V10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,9 +1108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1503,4 +1527,72 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>3013686313</v>
+      </c>
+      <c r="B2" s="3">
+        <v>904492748</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>3013684370</v>
+      </c>
+      <c r="B3" s="3">
+        <v>904492469</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3013688560</v>
+      </c>
+      <c r="B4" s="3">
+        <v>904493578</v>
+      </c>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3013686777</v>
+      </c>
+      <c r="B5" s="3">
+        <v>904493242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>3013686776</v>
+      </c>
+      <c r="B6" s="3">
+        <v>904493314</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update data for various tests
</commit_message>
<xml_diff>
--- a/Resources/1-Validation.xlsx
+++ b/Resources/1-Validation.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="195">
   <si>
     <t>Invoice No</t>
   </si>
@@ -596,6 +596,12 @@
   </si>
   <si>
     <t>1000006054</t>
+  </si>
+  <si>
+    <t>3013696912</t>
+  </si>
+  <si>
+    <t>1000004785</t>
   </si>
 </sst>
 </file>
@@ -1245,7 +1251,7 @@
         <v>49</v>
       </c>
       <c r="B1">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2">
@@ -1253,7 +1259,7 @@
         <v>50</v>
       </c>
       <c r="B2">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1263,7 +1269,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2420,6 +2426,20 @@
         <v>86</v>
       </c>
       <c r="D82" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>193</v>
+      </c>
+      <c r="B83" t="s">
+        <v>194</v>
+      </c>
+      <c r="C83">
+        <v>14010192017</v>
+      </c>
+      <c r="D83" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1-update schedule number and 2-data
</commit_message>
<xml_diff>
--- a/Resources/1-Validation.xlsx
+++ b/Resources/1-Validation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8115" activeTab="1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="229">
   <si>
     <t>Invoice No</t>
   </si>
@@ -698,6 +698,12 @@
   </si>
   <si>
     <t>1000006835</t>
+  </si>
+  <si>
+    <t>3013992465</t>
+  </si>
+  <si>
+    <t>1000007592</t>
   </si>
 </sst>
 </file>
@@ -1089,7 +1095,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1334,7 +1340,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1347,7 +1353,7 @@
         <v>49</v>
       </c>
       <c r="B1">
-        <v>59</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2">
@@ -1355,7 +1361,7 @@
         <v>50</v>
       </c>
       <c r="B2">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1365,7 +1371,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D115"/>
+  <dimension ref="A1:D116"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2984,6 +2990,20 @@
         <v>86</v>
       </c>
       <c r="D115" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s">
+        <v>227</v>
+      </c>
+      <c r="B116" t="s">
+        <v>228</v>
+      </c>
+      <c r="C116">
+        <v>17210192017</v>
+      </c>
+      <c r="D116" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2-update data and schedule number
</commit_message>
<xml_diff>
--- a/Resources/1-Validation.xlsx
+++ b/Resources/1-Validation.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="377">
   <si>
     <t>Invoice No</t>
   </si>
@@ -1064,6 +1064,90 @@
   </si>
   <si>
     <t>1000020458</t>
+  </si>
+  <si>
+    <t>3013974296</t>
+  </si>
+  <si>
+    <t>1000020465</t>
+  </si>
+  <si>
+    <t>3013905689</t>
+  </si>
+  <si>
+    <t>1000020466</t>
+  </si>
+  <si>
+    <t>3013905719</t>
+  </si>
+  <si>
+    <t>1000020467</t>
+  </si>
+  <si>
+    <t>3013981066</t>
+  </si>
+  <si>
+    <t>1000020468</t>
+  </si>
+  <si>
+    <t>3013998148</t>
+  </si>
+  <si>
+    <t>1000020469</t>
+  </si>
+  <si>
+    <t>3013245519</t>
+  </si>
+  <si>
+    <t>1000020470</t>
+  </si>
+  <si>
+    <t>3013527955</t>
+  </si>
+  <si>
+    <t>1000020471</t>
+  </si>
+  <si>
+    <t>3013898056</t>
+  </si>
+  <si>
+    <t>1000020472</t>
+  </si>
+  <si>
+    <t>1000020473</t>
+  </si>
+  <si>
+    <t>3013909121</t>
+  </si>
+  <si>
+    <t>1000020474</t>
+  </si>
+  <si>
+    <t>1000020475</t>
+  </si>
+  <si>
+    <t>3013913751</t>
+  </si>
+  <si>
+    <t>1000020476</t>
+  </si>
+  <si>
+    <t>3013914085</t>
+  </si>
+  <si>
+    <t>1000020477</t>
+  </si>
+  <si>
+    <t>3013901427</t>
+  </si>
+  <si>
+    <t>1000020478</t>
+  </si>
+  <si>
+    <t>3013997547</t>
+  </si>
+  <si>
+    <t>1000020482</t>
   </si>
 </sst>
 </file>
@@ -1713,7 +1797,7 @@
         <v>49</v>
       </c>
       <c r="B1">
-        <v>140</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2">
@@ -1721,7 +1805,7 @@
         <v>50</v>
       </c>
       <c r="B2">
-        <v>202</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -1731,7 +1815,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D201"/>
+  <dimension ref="A1:D216"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4554,6 +4638,216 @@
         <v>24010192017</v>
       </c>
       <c r="D201" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="s">
+        <v>349</v>
+      </c>
+      <c r="B202" t="s">
+        <v>350</v>
+      </c>
+      <c r="C202">
+        <v>24110192017</v>
+      </c>
+      <c r="D202" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="s">
+        <v>351</v>
+      </c>
+      <c r="B203" t="s">
+        <v>352</v>
+      </c>
+      <c r="C203">
+        <v>24210192017</v>
+      </c>
+      <c r="D203" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="s">
+        <v>353</v>
+      </c>
+      <c r="B204" t="s">
+        <v>354</v>
+      </c>
+      <c r="C204">
+        <v>24310192017</v>
+      </c>
+      <c r="D204" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="s">
+        <v>355</v>
+      </c>
+      <c r="B205" t="s">
+        <v>356</v>
+      </c>
+      <c r="C205">
+        <v>24410192017</v>
+      </c>
+      <c r="D205" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="s">
+        <v>357</v>
+      </c>
+      <c r="B206" t="s">
+        <v>358</v>
+      </c>
+      <c r="C206">
+        <v>24510192017</v>
+      </c>
+      <c r="D206" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="s">
+        <v>359</v>
+      </c>
+      <c r="B207" t="s">
+        <v>360</v>
+      </c>
+      <c r="C207">
+        <v>24610192017</v>
+      </c>
+      <c r="D207" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="s">
+        <v>361</v>
+      </c>
+      <c r="B208" t="s">
+        <v>362</v>
+      </c>
+      <c r="C208">
+        <v>24710192017</v>
+      </c>
+      <c r="D208" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="s">
+        <v>363</v>
+      </c>
+      <c r="B209" t="s">
+        <v>364</v>
+      </c>
+      <c r="C209">
+        <v>24810192017</v>
+      </c>
+      <c r="D209" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="s">
+        <v>353</v>
+      </c>
+      <c r="B210" t="s">
+        <v>365</v>
+      </c>
+      <c r="C210">
+        <v>24910192017</v>
+      </c>
+      <c r="D210" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="s">
+        <v>366</v>
+      </c>
+      <c r="B211" t="s">
+        <v>367</v>
+      </c>
+      <c r="C211">
+        <v>25010192017</v>
+      </c>
+      <c r="D211" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="s">
+        <v>366</v>
+      </c>
+      <c r="B212" t="s">
+        <v>368</v>
+      </c>
+      <c r="C212">
+        <v>25110192017</v>
+      </c>
+      <c r="D212" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="s">
+        <v>369</v>
+      </c>
+      <c r="B213" t="s">
+        <v>370</v>
+      </c>
+      <c r="C213">
+        <v>25210192017</v>
+      </c>
+      <c r="D213" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="s">
+        <v>371</v>
+      </c>
+      <c r="B214" t="s">
+        <v>372</v>
+      </c>
+      <c r="C214">
+        <v>25310192017</v>
+      </c>
+      <c r="D214" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="s">
+        <v>373</v>
+      </c>
+      <c r="B215" t="s">
+        <v>374</v>
+      </c>
+      <c r="C215">
+        <v>25410192017</v>
+      </c>
+      <c r="D215" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="s">
+        <v>375</v>
+      </c>
+      <c r="B216" t="s">
+        <v>376</v>
+      </c>
+      <c r="C216">
+        <v>25510192017</v>
+      </c>
+      <c r="D216" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>